<commit_message>
Deletes double-clicked selected row and Clear form
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,14 +429,14 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>Grade</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>Gender</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Grade</t>
-        </is>
-      </c>
       <c r="D1" t="inlineStr">
         <is>
           <t>OldSchool</t>
@@ -445,6 +445,87 @@
       <c r="E1" t="inlineStr">
         <is>
           <t>OldSchoolClass</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>789</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>dd</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>OldSchool B</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Geography</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>sdfsd</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>444</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>OldSchool A</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>History</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>joho</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2323</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>OldSchool B</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Art</t>
         </is>
       </c>
     </row>

</xml_diff>